<commit_message>
running version on beta test
</commit_message>
<xml_diff>
--- a/develop/initial suite/inputs.xlsx
+++ b/develop/initial suite/inputs.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_studio\wasim-2.0\develop\initial suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\284481c\Documents\R\wasim-2.0\develop\initial suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51831835-1605-4327-B461-8BB0939DDBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2CA3A3-8958-4E85-B255-AD25C7644E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Seq</t>
   </si>
@@ -34,24 +47,60 @@
     <t>loglevel</t>
   </si>
   <si>
-    <t>drawpoint_stock_max_stock</t>
-  </si>
-  <si>
-    <t>drawpoint_stock_init_stock</t>
-  </si>
-  <si>
-    <t>drawpoint_stock_access_limit</t>
+    <t>function () max(1, rnorm(1, 3600, 360))</t>
+  </si>
+  <si>
+    <t>function () max(1, rexp(1, rate = 1/(1 * 3600)))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 180, 18))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 120, 18))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 200, 5))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 60, 18))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 1800, 180))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 90, 9))</t>
+  </si>
+  <si>
+    <t>function() max(1, rnorm(1, 2400, 240))</t>
+  </si>
+  <si>
+    <t>lhd_travel_empty_delay</t>
+  </si>
+  <si>
+    <t>lhd_get_from_drawpoint_delay</t>
+  </si>
+  <si>
+    <t>drawpoint_max_stock</t>
+  </si>
+  <si>
+    <t>drawpoint_init_stock</t>
+  </si>
+  <si>
+    <t>drawpoint_access_limit</t>
+  </si>
+  <si>
+    <t>orepass_feed_hopper_max_stock</t>
+  </si>
+  <si>
+    <t>orepass_feed_hopper_init_stock</t>
+  </si>
+  <si>
+    <t>orepass_feed_hopper_access_limit</t>
   </si>
   <si>
     <t>orepass_stocks_max_stock</t>
   </si>
   <si>
-    <t>orepass_feed_hopper_init_stock</t>
-  </si>
-  <si>
-    <t>orepass_feed_hopper_access_limit</t>
-  </si>
-  <si>
     <t>orepass_stocks_init_stock</t>
   </si>
   <si>
@@ -67,92 +116,77 @@
     <t>hoist_stock_access_limit</t>
   </si>
   <si>
-    <t>n_lhds</t>
+    <t>n_lhd</t>
   </si>
   <si>
     <t>lhd_unit_capacity</t>
   </si>
   <si>
-    <t>lhd_travel_empty_delay</t>
-  </si>
-  <si>
-    <t>lhd_loads_from_drawpoint_Delay</t>
-  </si>
-  <si>
-    <t>lhd_travel_full_delay</t>
-  </si>
-  <si>
-    <t>n_trucks</t>
+    <t>lhd_mttr</t>
+  </si>
+  <si>
+    <t>lhd_mtbf</t>
+  </si>
+  <si>
+    <t>lhd_travel_loaded_delay</t>
+  </si>
+  <si>
+    <t>n_conveyor</t>
+  </si>
+  <si>
+    <t>conveyor_unit_capacity</t>
+  </si>
+  <si>
+    <t>conveyor_mttr</t>
+  </si>
+  <si>
+    <t>conveyor_mtbf</t>
+  </si>
+  <si>
+    <t>n_truck</t>
   </si>
   <si>
     <t>truck_unit_capacity</t>
   </si>
   <si>
+    <t>truck_mttr</t>
+  </si>
+  <si>
+    <t>truck_mtbf</t>
+  </si>
+  <si>
+    <t>truck_get_from_orepass_stocks_delay</t>
+  </si>
+  <si>
+    <t>truck_put_to_hoist_stock_delay</t>
+  </si>
+  <si>
+    <t>conveyor_travel_empty_delay</t>
+  </si>
+  <si>
+    <t>conveyor_travel_loaded_delay</t>
+  </si>
+  <si>
     <t>truck_travel_empty_delay</t>
   </si>
   <si>
-    <t>truck_loads_from_orepass_Delay</t>
-  </si>
-  <si>
-    <t>truck_travel_full_delay</t>
-  </si>
-  <si>
-    <t>truck_dumps_to_hoist_delay</t>
-  </si>
-  <si>
-    <t>function () max(1, rnorm(1, 3600, 360))</t>
-  </si>
-  <si>
-    <t>function () max(1, rexp(1, rate = 1/(1 * 3600)))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 180, 18))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 120, 18))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 200, 5))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 60, 18))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 1800, 180))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 90, 9))</t>
-  </si>
-  <si>
-    <t>function() max(1, rnorm(1, 2400, 240))</t>
-  </si>
-  <si>
-    <t>orepass_feed_hopper_max_stock</t>
-  </si>
-  <si>
-    <t>lhd_dumps_to_orepass_feed_hopper_delay</t>
-  </si>
-  <si>
-    <t>"function () max(1, rnorm(1, 3600, 360))"</t>
-  </si>
-  <si>
-    <t>lhd_mtbf</t>
-  </si>
-  <si>
-    <t>lhd_mttr</t>
-  </si>
-  <si>
-    <t>truck_mttr</t>
-  </si>
-  <si>
-    <t>truck_mtbf</t>
+    <t>truck_travel_loaded_delay</t>
+  </si>
+  <si>
+    <t>lhd_put_to_orepass_feed_hopper_delay</t>
+  </si>
+  <si>
+    <t>conveyor_get_from_orepass_feed_hopper_delay</t>
+  </si>
+  <si>
+    <t>conveyor_put_to_orepass_stocks_delay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +320,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -629,8 +669,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -986,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AM5" sqref="AM5:AM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1040,7 @@
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -1012,21 +1053,27 @@
     <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.28515625" customWidth="1"/>
     <col min="20" max="20" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="33" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="32" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="38" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="42" customWidth="1"/>
     <col min="31" max="31" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="31" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="37" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="36" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1040,91 +1087,115 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AK1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AM1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN1" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1147,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1159,13 +1230,14 @@
         <v>1000</v>
       </c>
       <c r="L2">
+        <f>K2/2</f>
         <v>500</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2">
-        <v>9999999</v>
+        <v>999999999</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -1180,22 +1252,22 @@
         <v>21</v>
       </c>
       <c r="S2" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="T2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="U2" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="V2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="W2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="X2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="Y2">
         <v>1</v>
@@ -1204,25 +1276,49 @@
         <v>64</v>
       </c>
       <c r="AA2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="AC2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="AD2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="AE2" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="AF2" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>64</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1236,91 +1332,163 @@
         <v>1</v>
       </c>
       <c r="E3">
+        <f t="shared" ref="E3:H3" si="0">E2</f>
         <v>9999999</v>
       </c>
       <c r="F3">
+        <f t="shared" si="0"/>
         <v>9999999</v>
       </c>
       <c r="G3">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H3">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="I3">
+        <f>I2</f>
         <v>0</v>
       </c>
       <c r="J3">
+        <f>J2</f>
         <v>1</v>
       </c>
       <c r="K3">
+        <f>K2</f>
         <v>1000</v>
       </c>
       <c r="L3">
+        <f>K3/2</f>
         <v>500</v>
       </c>
       <c r="M3">
+        <f>M2</f>
         <v>1</v>
       </c>
       <c r="N3">
-        <v>9999999</v>
+        <f>N2</f>
+        <v>999999999</v>
       </c>
       <c r="O3">
+        <f>O2</f>
         <v>0</v>
       </c>
       <c r="P3">
+        <f>P2</f>
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3">
+        <f>R2</f>
         <v>21</v>
       </c>
-      <c r="S3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" t="s">
-        <v>31</v>
+      <c r="S3" t="str">
+        <f>S2</f>
+        <v>function () max(1, rexp(1, rate = 1/(1 * 3600)))</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:AF3" si="1">T2</f>
+        <v>function () max(1, rexp(1, rate = 1/(1 * 3600)))</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 180, 18))</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 120, 18))</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 200, 5))</v>
+      </c>
+      <c r="X3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 60, 18))</v>
       </c>
       <c r="Y3">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Z3">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="AA3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>33</v>
+      <c r="AA3" t="str">
+        <f t="shared" si="1"/>
+        <v>function () max(1, rnorm(1, 3600, 360))</v>
+      </c>
+      <c r="AB3" t="str">
+        <f t="shared" si="1"/>
+        <v>function () max(1, rexp(1, rate = 1/(1 * 3600)))</v>
+      </c>
+      <c r="AC3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 1800, 180))</v>
+      </c>
+      <c r="AD3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 90, 9))</v>
+      </c>
+      <c r="AE3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 2400, 240))</v>
+      </c>
+      <c r="AF3" t="str">
+        <f t="shared" si="1"/>
+        <v>function() max(1, rnorm(1, 90, 9))</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" ref="AG3" si="2">AG2</f>
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" ref="AH3" si="3">AH2</f>
+        <v>64</v>
+      </c>
+      <c r="AI3" t="str">
+        <f t="shared" ref="AI3" si="4">AI2</f>
+        <v>function () max(1, rnorm(1, 3600, 360))</v>
+      </c>
+      <c r="AJ3" t="str">
+        <f t="shared" ref="AJ3" si="5">AJ2</f>
+        <v>function () max(1, rexp(1, rate = 1/(1 * 3600)))</v>
+      </c>
+      <c r="AK3" t="str">
+        <f t="shared" ref="AK3" si="6">AK2</f>
+        <v>function() max(1, rnorm(1, 1800, 180))</v>
+      </c>
+      <c r="AL3" t="str">
+        <f t="shared" ref="AL3" si="7">AL2</f>
+        <v>function() max(1, rnorm(1, 90, 9))</v>
+      </c>
+      <c r="AM3" t="str">
+        <f t="shared" ref="AM3" si="8">AM2</f>
+        <v>function() max(1, rnorm(1, 2400, 240))</v>
+      </c>
+      <c r="AN3" t="str">
+        <f t="shared" ref="AN3" si="9">AN2</f>
+        <v>function() max(1, rnorm(1, 90, 9))</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="22" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <f>448/AH2</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>